<commit_message>
Update NSW vaccination to 2021-08-01.
</commit_message>
<xml_diff>
--- a/NSW/input/pop_essential_2007.xlsx
+++ b/NSW/input/pop_essential_2007.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Repos\CovidABM\NSW\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{066A1E88-591D-4B54-9E51-18EF001724F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC3C247-DCE4-4740-9E9A-DECF5E25F033}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pop_essential_2007_bau" sheetId="1" r:id="rId1"/>
     <sheet name="AZ splitter" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="72">
   <si>
     <t>totalAgents</t>
   </si>
@@ -226,11 +237,23 @@
   <si>
     <t>AZ top ess</t>
   </si>
+  <si>
+    <t>Tweak</t>
+  </si>
+  <si>
+    <t>prog</t>
+  </si>
+  <si>
+    <t>vac</t>
+  </si>
+  <si>
+    <t>vacBase</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1067,11 +1090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AJ43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z31" sqref="Z31"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,16 +1103,18 @@
     <col min="9" max="13" width="3.140625" customWidth="1"/>
     <col min="21" max="21" width="32" customWidth="1"/>
     <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" customWidth="1"/>
-    <col min="24" max="26" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" customWidth="1"/>
-    <col min="29" max="29" width="10.28515625" customWidth="1"/>
-    <col min="30" max="30" width="11.42578125" customWidth="1"/>
-    <col min="32" max="32" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" customWidth="1"/>
+    <col min="29" max="29" width="9" customWidth="1"/>
+    <col min="30" max="32" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9" customWidth="1"/>
+    <col min="35" max="35" width="10.28515625" customWidth="1"/>
+    <col min="36" max="36" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1154,31 +1179,34 @@
         <v>20</v>
       </c>
       <c r="X1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1">
+        <v>8166000</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" t="s">
         <v>60</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AE1" t="s">
         <v>61</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AF1" t="s">
         <v>62</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AG1" t="s">
         <v>59</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AI1" t="s">
         <v>45</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AJ1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AG1">
-        <v>8166000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>82</v>
       </c>
@@ -1219,6 +1247,7 @@
         <v>1</v>
       </c>
       <c r="N2">
+        <f>IF(SUM(AD2:AG2) &gt;0,ROUND(AB2*(AD2*$Y$26+AE2*$Y$27+AF2*$Y$28+AG2*$Y$29)/SUM(AD2:AG2),0), 0)</f>
         <v>58</v>
       </c>
       <c r="O2">
@@ -1245,42 +1274,45 @@
       <c r="V2" t="s">
         <v>65</v>
       </c>
-      <c r="W2" t="str">
+      <c r="X2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2">
+        <v>2327237</v>
+      </c>
+      <c r="AB2">
+        <v>58</v>
+      </c>
+      <c r="AC2" t="str">
         <f>IF(N2&gt;A2,"WARN","")</f>
         <v/>
       </c>
-      <c r="X2">
+      <c r="AD2">
         <f>IF(B2&gt;20,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Y2">
-        <f>IF(B2&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z2">
+      <c r="AE2">
+        <f t="shared" ref="AE2:AE28" si="0">IF(B2&gt;50,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF2">
         <f>IF(B2&gt;70,1,0)</f>
         <v>1</v>
       </c>
-      <c r="AA2">
+      <c r="AG2">
         <f>IF(U2="Top essential workers",1,0)</f>
         <v>0</v>
       </c>
-      <c r="AC2" s="1">
-        <f>N2</f>
+      <c r="AI2" s="1">
+        <f t="shared" ref="AI2:AI8" si="1">N2</f>
         <v>58</v>
       </c>
-      <c r="AD2" s="1">
-        <f>(P2-1)/P2*N2</f>
+      <c r="AJ2" s="1">
+        <f t="shared" ref="AJ2:AJ8" si="2">(P2-1)/P2*N2</f>
         <v>27.473684210526315</v>
       </c>
-      <c r="AF2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2">
-        <v>2327237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -1321,6 +1353,7 @@
         <v>1</v>
       </c>
       <c r="N3">
+        <f>IF(SUM(AD3:AG3) &gt;0,ROUND(AB3*(AD3*$Y$26+AE3*$Y$27+AF3*$Y$28+AG3*$Y$29)/SUM(AD3:AG3),0), 0)</f>
         <v>16</v>
       </c>
       <c r="O3">
@@ -1345,44 +1378,47 @@
         <v>26</v>
       </c>
       <c r="V3">
-        <v>0.25</v>
-      </c>
-      <c r="W3" t="str">
-        <f t="shared" ref="W3:W42" si="0">IF(N3&gt;A3,"WARN","")</f>
+        <v>0</v>
+      </c>
+      <c r="X3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y3">
+        <v>948667</v>
+      </c>
+      <c r="AB3">
+        <v>16</v>
+      </c>
+      <c r="AC3" t="str">
+        <f>IF(N3&gt;A3,"WARN","")</f>
         <v/>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X28" si="1">IF(B3&gt;20,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <f>IF(B3&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z3">
-        <f t="shared" ref="Z3:Z28" si="2">IF(B3&gt;70,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AA3">
-        <f t="shared" ref="AA3:AA28" si="3">IF(U3="Top essential workers",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1">
-        <f>N3</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD28" si="3">IF(B3&gt;20,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" ref="AF3:AF28" si="4">IF(B3&gt;70,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" ref="AG3:AG28" si="5">IF(U3="Top essential workers",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI3" s="1">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="AD3" s="1">
-        <f>(P3-1)/P3*N3</f>
+      <c r="AJ3" s="1">
+        <f t="shared" si="2"/>
         <v>9.6254980079681278</v>
       </c>
-      <c r="AF3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG3">
-        <v>948667</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1423,6 +1459,7 @@
         <v>1</v>
       </c>
       <c r="N4">
+        <f>IF(SUM(AD4:AG4) &gt;0,ROUND(AB4*(AD4*$Y$26+AE4*$Y$27+AF4*$Y$28+AG4*$Y$29)/SUM(AD4:AG4),0), 0)</f>
         <v>0</v>
       </c>
       <c r="O4">
@@ -1449,39 +1486,42 @@
       <c r="V4" t="s">
         <v>66</v>
       </c>
-      <c r="W4" t="str">
+      <c r="Y4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="str">
+        <f>IF(N4&gt;A4,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE4">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI4" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y4">
-        <f>IF(B4&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC4" s="1">
-        <f>N4</f>
-        <v>0</v>
-      </c>
-      <c r="AD4" s="1">
-        <f>(P4-1)/P4*N4</f>
-        <v>0</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1522,6 +1562,7 @@
         <v>1</v>
       </c>
       <c r="N5">
+        <f>IF(SUM(AD5:AG5) &gt;0,ROUND(AB5*(AD5*$Y$26+AE5*$Y$27+AF5*$Y$28+AG5*$Y$29)/SUM(AD5:AG5),0), 0)</f>
         <v>3</v>
       </c>
       <c r="O5">
@@ -1546,45 +1587,48 @@
         <v>24</v>
       </c>
       <c r="V5">
-        <v>0.25</v>
-      </c>
-      <c r="W5" t="str">
+        <v>0</v>
+      </c>
+      <c r="X5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y5" s="2">
+        <f>Y2/Y1-Y6</f>
+        <v>0.16881827087925544</v>
+      </c>
+      <c r="AB5">
+        <v>3</v>
+      </c>
+      <c r="AC5" t="str">
+        <f>IF(N5&gt;A5,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE5">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <f>IF(B5&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z5">
+        <v>3</v>
+      </c>
+      <c r="AJ5" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="1">
-        <f>N5</f>
-        <v>3</v>
-      </c>
-      <c r="AD5" s="1">
-        <f>(P5-1)/P5*N5</f>
         <v>0.90209790209790208</v>
       </c>
-      <c r="AF5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG5" s="2">
-        <f>AG2/AG1-AG6</f>
-        <v>0.16881827087925544</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -1625,6 +1669,7 @@
         <v>1</v>
       </c>
       <c r="N6">
+        <f>IF(SUM(AD6:AG6) &gt;0,ROUND(AB6*(AD6*$Y$26+AE6*$Y$27+AF6*$Y$28+AG6*$Y$29)/SUM(AD6:AG6),0), 0)</f>
         <v>6</v>
       </c>
       <c r="O6">
@@ -1651,43 +1696,46 @@
       <c r="V6" t="s">
         <v>67</v>
       </c>
-      <c r="W6" t="str">
+      <c r="X6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y6" s="2">
+        <f>Y3/Y1</f>
+        <v>0.11617278961547882</v>
+      </c>
+      <c r="AB6">
+        <v>6</v>
+      </c>
+      <c r="AC6" t="str">
+        <f>IF(N6&gt;A6,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE6">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y6">
-        <f>IF(B6&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z6">
+        <v>6</v>
+      </c>
+      <c r="AJ6" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="1">
-        <f>N6</f>
-        <v>6</v>
-      </c>
-      <c r="AD6" s="1">
-        <f>(P6-1)/P6*N6</f>
         <v>1.5555555555555558</v>
       </c>
-      <c r="AF6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG6" s="2">
-        <f>AG3/AG1</f>
-        <v>0.11617278961547882</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>256</v>
       </c>
@@ -1728,6 +1776,7 @@
         <v>1</v>
       </c>
       <c r="N7">
+        <f>IF(SUM(AD7:AG7) &gt;0,ROUND(AB7*(AD7*$Y$26+AE7*$Y$27+AF7*$Y$28+AG7*$Y$29)/SUM(AD7:AG7),0), 0)</f>
         <v>157</v>
       </c>
       <c r="O7">
@@ -1752,38 +1801,41 @@
         <v>29</v>
       </c>
       <c r="V7">
-        <v>0.25</v>
-      </c>
-      <c r="W7" t="str">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>157</v>
+      </c>
+      <c r="AC7" t="str">
+        <f>IF(N7&gt;A7,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE7">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y7">
-        <f>IF(B7&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z7">
+        <v>157</v>
+      </c>
+      <c r="AJ7" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="1">
-        <f>N7</f>
-        <v>157</v>
-      </c>
-      <c r="AD7" s="1">
-        <f>(P7-1)/P7*N7</f>
         <v>47.209790209790206</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>31</v>
       </c>
@@ -1824,6 +1876,7 @@
         <v>1</v>
       </c>
       <c r="N8">
+        <f>IF(SUM(AD8:AG8) &gt;0,ROUND(AB8*(AD8*$Y$26+AE8*$Y$27+AF8*$Y$28+AG8*$Y$29)/SUM(AD8:AG8),0), 0)</f>
         <v>19</v>
       </c>
       <c r="O8">
@@ -1847,39 +1900,42 @@
       <c r="U8" t="s">
         <v>28</v>
       </c>
-      <c r="W8" t="str">
+      <c r="Y8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB8">
+        <v>19</v>
+      </c>
+      <c r="AC8" t="str">
+        <f>IF(N8&gt;A8,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE8">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="1">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y8">
-        <f>IF(B8&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z8">
+        <v>19</v>
+      </c>
+      <c r="AJ8" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC8" s="1">
-        <f>N8</f>
-        <v>19</v>
-      </c>
-      <c r="AD8" s="1">
-        <f>(P8-1)/P8*N8</f>
         <v>5.7132867132867124</v>
       </c>
-      <c r="AG8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>180</v>
       </c>
@@ -1920,6 +1976,7 @@
         <v>1</v>
       </c>
       <c r="N9">
+        <f>IF(SUM(AD9:AG9) &gt;0,ROUND(AB9*(AD9*$Y$26+AE9*$Y$27+AF9*$Y$28+AG9*$Y$29)/SUM(AD9:AG9),0), 0)</f>
         <v>136</v>
       </c>
       <c r="O9">
@@ -1943,43 +2000,46 @@
       <c r="U9" t="s">
         <v>30</v>
       </c>
-      <c r="W9" t="str">
+      <c r="X9" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y9" s="2">
+        <f>SUM(AI2:AI42)/2500-Y10</f>
+        <v>0.16290596082955267</v>
+      </c>
+      <c r="AB9">
+        <v>136</v>
+      </c>
+      <c r="AC9" t="str">
+        <f>IF(N9&gt;A9,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X9">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y9">
-        <f>IF(B9&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z9">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC9" s="1">
-        <f t="shared" ref="AC9:AC28" si="4">N9</f>
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="1">
+        <f t="shared" ref="AI9:AI28" si="6">N9</f>
         <v>136</v>
       </c>
-      <c r="AD9" s="1">
-        <f t="shared" ref="AD9:AD28" si="5">(P9-1)/P9*N9</f>
+      <c r="AJ9" s="1">
+        <f t="shared" ref="AJ9:AJ28" si="7">(P9-1)/P9*N9</f>
         <v>59.59550561797753</v>
       </c>
-      <c r="AF9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG9" s="2">
-        <f>SUM(AC2:AC42)/2500-AG10</f>
-        <v>0.16790596082955267</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>120</v>
       </c>
@@ -2020,6 +2080,7 @@
         <v>1</v>
       </c>
       <c r="N10">
+        <f>IF(SUM(AD10:AG10) &gt;0,ROUND(AB10*(AD10*$Y$26+AE10*$Y$27+AF10*$Y$28+AG10*$Y$29)/SUM(AD10:AG10),0), 0)</f>
         <v>53</v>
       </c>
       <c r="O10">
@@ -2043,46 +2104,49 @@
       <c r="U10" t="s">
         <v>31</v>
       </c>
-      <c r="W10" t="str">
+      <c r="X10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y10" s="2">
+        <f>SUM(AJ2:AJ42)/2500</f>
+        <v>0.11149403917044733</v>
+      </c>
+      <c r="AB10">
+        <v>53</v>
+      </c>
+      <c r="AC10" t="str">
+        <f>IF(N10&gt;A10,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE10">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y10">
-        <f>IF(B10&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF10">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI10" s="1">
+        <f t="shared" si="6"/>
         <v>53</v>
       </c>
-      <c r="AD10" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ10" s="1">
+        <f t="shared" si="7"/>
         <v>13.740740740740742</v>
       </c>
-      <c r="AF10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG10" s="2">
-        <f>SUM(AD2:AD42)/2500</f>
-        <v>0.11169403917044733</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>'AZ splitter'!A11-'AZ splitter'!A39</f>
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="B11">
         <v>55</v>
@@ -2099,7 +2163,7 @@
       </c>
       <c r="F11">
         <f>'AZ splitter'!F11-'AZ splitter'!F39</f>
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -2123,6 +2187,7 @@
         <v>1</v>
       </c>
       <c r="N11">
+        <f>IF(SUM(AD11:AG11) &gt;0,ROUND(AB11*(AD11*$Y$26+AE11*$Y$27+AF11*$Y$28+AG11*$Y$29)/SUM(AD11:AG11),0), 0)</f>
         <v>76</v>
       </c>
       <c r="O11">
@@ -2149,39 +2214,42 @@
       <c r="V11" t="s">
         <v>63</v>
       </c>
-      <c r="W11" t="str">
+      <c r="AB11">
+        <v>76</v>
+      </c>
+      <c r="AC11" t="str">
+        <f>IF(N11&gt;A11,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE11">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X11">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y11">
-        <f>IF(B11&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF11">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="1">
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
-      <c r="AD11" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ11" s="1">
+        <f t="shared" si="7"/>
         <v>19.703703703703706</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>'AZ splitter'!A12-'AZ splitter'!A40</f>
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>25</v>
@@ -2194,11 +2262,11 @@
       </c>
       <c r="E12">
         <f>'AZ splitter'!E12-'AZ splitter'!E40</f>
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="F12">
         <f>'AZ splitter'!F12-'AZ splitter'!F40</f>
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2222,6 +2290,7 @@
         <v>1</v>
       </c>
       <c r="N12">
+        <f>IF(SUM(AD12:AG12) &gt;0,ROUND(AB12*(AD12*$Y$26+AE12*$Y$27+AF12*$Y$28+AG12*$Y$29)/SUM(AD12:AG12),0), 0)</f>
         <v>29</v>
       </c>
       <c r="O12">
@@ -2249,39 +2318,44 @@
         <f>SUM(A:A)</f>
         <v>2500</v>
       </c>
-      <c r="W12" t="str">
+      <c r="W12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12">
+        <v>29</v>
+      </c>
+      <c r="AC12" t="str">
+        <f>IF(N12&gt;A12,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE12">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X12">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y12">
-        <f>IF(B12&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF12">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AI12" s="1">
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="AD12" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ12" s="1">
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>'AZ splitter'!A13-'AZ splitter'!A41</f>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>35</v>
@@ -2294,11 +2368,11 @@
       </c>
       <c r="E13">
         <f>'AZ splitter'!E13-'AZ splitter'!E41</f>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="F13">
         <f>'AZ splitter'!F13-'AZ splitter'!F41</f>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -2322,6 +2396,7 @@
         <v>1</v>
       </c>
       <c r="N13">
+        <f>IF(SUM(AD13:AG13) &gt;0,ROUND(AB13*(AD13*$Y$26+AE13*$Y$27+AF13*$Y$28+AG13*$Y$29)/SUM(AD13:AG13),0), 0)</f>
         <v>22</v>
       </c>
       <c r="O13">
@@ -2345,48 +2420,51 @@
       <c r="U13" t="s">
         <v>44</v>
       </c>
-      <c r="W13" t="str">
+      <c r="X13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB13">
+        <v>22</v>
+      </c>
+      <c r="AC13" t="str">
+        <f>IF(N13&gt;A13,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE13">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y13">
-        <f>IF(B13&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AC13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF13">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AI13" s="1">
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="AD13" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ13" s="1">
+        <f t="shared" si="7"/>
         <v>14.413793103448276</v>
       </c>
-      <c r="AF13" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>'AZ splitter'!A14-'AZ splitter'!A42</f>
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B14">
         <v>45</v>
@@ -2399,11 +2477,11 @@
       </c>
       <c r="E14">
         <f>'AZ splitter'!E14-'AZ splitter'!E42</f>
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="F14">
         <f>'AZ splitter'!F14-'AZ splitter'!F42</f>
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -2427,6 +2505,7 @@
         <v>1</v>
       </c>
       <c r="N14">
+        <f>IF(SUM(AD14:AG14) &gt;0,ROUND(AB14*(AD14*$Y$26+AE14*$Y$27+AF14*$Y$28+AG14*$Y$29)/SUM(AD14:AG14),0), 0)</f>
         <v>23</v>
       </c>
       <c r="O14">
@@ -2453,48 +2532,51 @@
       <c r="V14" t="s">
         <v>64</v>
       </c>
-      <c r="W14" t="str">
+      <c r="X14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0.35449999999999998</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="AB14">
+        <v>23</v>
+      </c>
+      <c r="AC14" t="str">
+        <f>IF(N14&gt;A14,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE14">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X14">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y14">
-        <f>IF(B14&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="AC14" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF14">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AI14" s="1">
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="AD14" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ14" s="1">
+        <f t="shared" si="7"/>
         <v>15.068965517241379</v>
       </c>
-      <c r="AF14" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG14" s="2">
-        <v>0.35449999999999998</v>
-      </c>
-      <c r="AH14" s="2">
-        <v>0.14449999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>'AZ splitter'!A15-'AZ splitter'!A43</f>
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B15">
         <v>25</v>
@@ -2511,7 +2593,7 @@
       </c>
       <c r="F15">
         <f>'AZ splitter'!F15-'AZ splitter'!F43</f>
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -2535,6 +2617,7 @@
         <v>1</v>
       </c>
       <c r="N15">
+        <f>IF(SUM(AD15:AG15) &gt;0,ROUND(AB15*(AD15*$Y$26+AE15*$Y$27+AF15*$Y$28+AG15*$Y$29)/SUM(AD15:AG15),0), 0)</f>
         <v>6</v>
       </c>
       <c r="O15">
@@ -2560,50 +2643,53 @@
       </c>
       <c r="V15">
         <f>SUM(N:N)</f>
-        <v>699</v>
-      </c>
-      <c r="W15" t="str">
+        <v>686</v>
+      </c>
+      <c r="X15" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0.58779999999999999</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>0.2087</v>
+      </c>
+      <c r="AB15">
+        <v>6</v>
+      </c>
+      <c r="AC15" t="str">
+        <f>IF(N15&gt;A15,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE15">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y15">
-        <f>IF(B15&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC15" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF15">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI15" s="1">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="AD15" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ15" s="1">
+        <f t="shared" si="7"/>
         <v>2.9696969696969697</v>
       </c>
-      <c r="AF15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG15" s="2">
-        <v>0.58779999999999999</v>
-      </c>
-      <c r="AH15" s="2">
-        <v>0.2087</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>'AZ splitter'!A16-'AZ splitter'!A44</f>
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>35</v>
@@ -2620,7 +2706,7 @@
       </c>
       <c r="F16">
         <f>'AZ splitter'!F16-'AZ splitter'!F44</f>
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G16">
         <v>2</v>
@@ -2644,6 +2730,7 @@
         <v>1</v>
       </c>
       <c r="N16">
+        <f>IF(SUM(AD16:AG16) &gt;0,ROUND(AB16*(AD16*$Y$26+AE16*$Y$27+AF16*$Y$28+AG16*$Y$29)/SUM(AD16:AG16),0), 0)</f>
         <v>9</v>
       </c>
       <c r="O16">
@@ -2667,48 +2754,51 @@
       <c r="U16" t="s">
         <v>35</v>
       </c>
-      <c r="W16" t="str">
+      <c r="X16" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0.74609999999999999</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>0.34189999999999998</v>
+      </c>
+      <c r="AB16">
+        <v>9</v>
+      </c>
+      <c r="AC16" t="str">
+        <f>IF(N16&gt;A16,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE16">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X16">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y16">
-        <f>IF(B16&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF16">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="1">
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="AD16" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ16" s="1">
+        <f t="shared" si="7"/>
         <v>4.5882352941176467</v>
       </c>
-      <c r="AF16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG16" s="2">
-        <v>0.74609999999999999</v>
-      </c>
-      <c r="AH16" s="2">
-        <v>0.34189999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>'AZ splitter'!A17-'AZ splitter'!A45</f>
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>45</v>
@@ -2725,7 +2815,7 @@
       </c>
       <c r="F17">
         <f>'AZ splitter'!F17-'AZ splitter'!F45</f>
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -2749,6 +2839,7 @@
         <v>1</v>
       </c>
       <c r="N17">
+        <f>IF(SUM(AD17:AG17) &gt;0,ROUND(AB17*(AD17*$Y$26+AE17*$Y$27+AF17*$Y$28+AG17*$Y$29)/SUM(AD17:AG17),0), 0)</f>
         <v>13</v>
       </c>
       <c r="O17">
@@ -2772,46 +2863,49 @@
       <c r="U17" t="s">
         <v>36</v>
       </c>
-      <c r="W17" t="str">
+      <c r="X17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="Z17" s="2"/>
+      <c r="AB17">
+        <v>13</v>
+      </c>
+      <c r="AC17" t="str">
+        <f>IF(N17&gt;A17,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE17">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X17">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y17">
-        <f>IF(B17&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC17" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF17">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI17" s="1">
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="AD17" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ17" s="1">
+        <f t="shared" si="7"/>
         <v>6.6585365853658534</v>
       </c>
-      <c r="AF17" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG17" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="AH17" s="2"/>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>'AZ splitter'!A18-'AZ splitter'!A46</f>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>55</v>
@@ -2828,7 +2922,7 @@
       </c>
       <c r="F18">
         <f>'AZ splitter'!F18-'AZ splitter'!F46</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G18">
         <v>2</v>
@@ -2852,6 +2946,7 @@
         <v>1</v>
       </c>
       <c r="N18">
+        <f>IF(SUM(AD18:AG18) &gt;0,ROUND(AB18*(AD18*$Y$26+AE18*$Y$27+AF18*$Y$28+AG18*$Y$29)/SUM(AD18:AG18),0), 0)</f>
         <v>11</v>
       </c>
       <c r="O18">
@@ -2875,41 +2970,44 @@
       <c r="U18" t="s">
         <v>27</v>
       </c>
-      <c r="W18" t="str">
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AB18">
+        <v>11</v>
+      </c>
+      <c r="AC18" t="str">
+        <f>IF(N18&gt;A18,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE18">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y18">
-        <f>IF(B18&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF18">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI18" s="1">
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
-      <c r="AD18" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ18" s="1">
+        <f t="shared" si="7"/>
         <v>2.8518518518518521</v>
       </c>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>'AZ splitter'!A19-'AZ splitter'!A47</f>
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="B19">
         <v>25</v>
@@ -2926,7 +3024,7 @@
       </c>
       <c r="F19">
         <f>'AZ splitter'!F19-'AZ splitter'!F47</f>
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="G19">
         <v>3</v>
@@ -2950,6 +3048,7 @@
         <v>1</v>
       </c>
       <c r="N19">
+        <f>IF(SUM(AD19:AG19) &gt;0,ROUND(AB19*(AD19*$Y$26+AE19*$Y$27+AF19*$Y$28+AG19*$Y$29)/SUM(AD19:AG19),0), 0)</f>
         <v>0</v>
       </c>
       <c r="O19">
@@ -2973,48 +3072,51 @@
       <c r="U19" t="s">
         <v>37</v>
       </c>
-      <c r="W19" t="str">
+      <c r="X19" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="str">
+        <f>IF(N19&gt;A19,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE19">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X19">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y19">
-        <f>IF(B19&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD19" s="1">
+      <c r="AG19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AF19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI19" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>'AZ splitter'!A20-'AZ splitter'!A48</f>
-        <v>142</v>
+        <v>189</v>
       </c>
       <c r="B20">
         <v>35</v>
@@ -3031,7 +3133,7 @@
       </c>
       <c r="F20">
         <f>'AZ splitter'!F20-'AZ splitter'!F48</f>
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="G20">
         <v>3</v>
@@ -3055,6 +3157,7 @@
         <v>1</v>
       </c>
       <c r="N20">
+        <f>IF(SUM(AD20:AG20) &gt;0,ROUND(AB20*(AD20*$Y$26+AE20*$Y$27+AF20*$Y$28+AG20*$Y$29)/SUM(AD20:AG20),0), 0)</f>
         <v>0</v>
       </c>
       <c r="O20">
@@ -3078,50 +3181,53 @@
       <c r="U20" t="s">
         <v>38</v>
       </c>
-      <c r="W20" t="str">
+      <c r="X20" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y20" s="2">
+        <f>SUMPRODUCT(AI:AI,AD:AD)/SUMPRODUCT(A:A,AD:AD)</f>
+        <v>0.3521560574948665</v>
+      </c>
+      <c r="Z20" s="2">
+        <f>SUMPRODUCT(AJ:AJ,AD:AD)/SUMPRODUCT(A:A,AD:AD)</f>
+        <v>0.14308783261094371</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20" t="str">
+        <f>IF(N20&gt;A20,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE20">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X20">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y20">
-        <f>IF(B20&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF20">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD20" s="1">
+      <c r="AG20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AF20" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG20" s="2">
-        <f>SUMPRODUCT(AC:AC,X:X)/SUMPRODUCT(A:A,X:X)</f>
-        <v>0.41854789505796219</v>
-      </c>
-      <c r="AH20" s="2">
-        <f>SUMPRODUCT(AD:AD,X:X)/SUMPRODUCT(A:A,X:X)</f>
-        <v>0.17006412320080436</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI20" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>'AZ splitter'!A21-'AZ splitter'!A49</f>
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="B21">
         <v>45</v>
@@ -3138,7 +3244,7 @@
       </c>
       <c r="F21">
         <f>'AZ splitter'!F21-'AZ splitter'!F49</f>
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="G21">
         <v>3</v>
@@ -3162,6 +3268,7 @@
         <v>1</v>
       </c>
       <c r="N21">
+        <f>IF(SUM(AD21:AG21) &gt;0,ROUND(AB21*(AD21*$Y$26+AE21*$Y$27+AF21*$Y$28+AG21*$Y$29)/SUM(AD21:AG21),0), 0)</f>
         <v>29</v>
       </c>
       <c r="O21">
@@ -3185,50 +3292,53 @@
       <c r="U21" t="s">
         <v>39</v>
       </c>
-      <c r="W21" t="str">
+      <c r="X21" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y21" s="2">
+        <f>SUMPRODUCT(AI:AI,AE:AE)/SUMPRODUCT(A:A,AE:AE)</f>
+        <v>0.58797814207650279</v>
+      </c>
+      <c r="Z21" s="2">
+        <f>SUMPRODUCT(AJ:AJ,AE:AE)/SUMPRODUCT(A:A,AE:AE)</f>
+        <v>0.20769866763407657</v>
+      </c>
+      <c r="AB21">
+        <v>29</v>
+      </c>
+      <c r="AC21" t="str">
+        <f>IF(N21&gt;A21,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE21">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X21">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y21">
-        <f>IF(B21&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF21">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI21" s="1">
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="AD21" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ21" s="1">
+        <f t="shared" si="7"/>
         <v>14.853658536585366</v>
       </c>
-      <c r="AF21" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG21" s="2">
-        <f>SUMPRODUCT(AC:AC,Y:Y)/SUMPRODUCT(A:A,Y:Y)</f>
-        <v>0.62268518518518523</v>
-      </c>
-      <c r="AH21" s="2">
-        <f>SUMPRODUCT(AD:AD,Y:Y)/SUMPRODUCT(A:A,Y:Y)</f>
-        <v>0.21995865843192136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>'AZ splitter'!A22-'AZ splitter'!A50</f>
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <v>25</v>
@@ -3241,11 +3351,11 @@
       </c>
       <c r="E22">
         <f>'AZ splitter'!E22-'AZ splitter'!E50</f>
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F22">
         <f>'AZ splitter'!F22-'AZ splitter'!F50</f>
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G22">
         <v>3</v>
@@ -3269,6 +3379,7 @@
         <v>1</v>
       </c>
       <c r="N22">
+        <f>IF(SUM(AD22:AG22) &gt;0,ROUND(AB22*(AD22*$Y$26+AE22*$Y$27+AF22*$Y$28+AG22*$Y$29)/SUM(AD22:AG22),0), 0)</f>
         <v>7</v>
       </c>
       <c r="O22">
@@ -3292,50 +3403,53 @@
       <c r="U22" t="s">
         <v>40</v>
       </c>
-      <c r="W22" t="str">
+      <c r="X22" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y22" s="2">
+        <f>SUMPRODUCT(AI:AI,AF:AF)/SUMPRODUCT(A:A,AF:AF)</f>
+        <v>0.74468085106382975</v>
+      </c>
+      <c r="Z22" s="2">
+        <f>SUMPRODUCT(AJ:AJ,AF:AF)/SUMPRODUCT(A:A,AF:AF)</f>
+        <v>0.34288896395912044</v>
+      </c>
+      <c r="AB22">
+        <v>7</v>
+      </c>
+      <c r="AC22" t="str">
+        <f>IF(N22&gt;A22,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE22">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X22">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y22">
-        <f>IF(B22&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF22">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="1">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="AD22" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ22" s="1">
+        <f t="shared" si="7"/>
         <v>4.5862068965517242</v>
       </c>
-      <c r="AF22" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG22" s="2">
-        <f>SUMPRODUCT(AC:AC,Z:Z)/SUMPRODUCT(A:A,Z:Z)</f>
-        <v>0.74468085106382975</v>
-      </c>
-      <c r="AH22" s="2">
-        <f>SUMPRODUCT(AD:AD,Z:Z)/SUMPRODUCT(A:A,Z:Z)</f>
-        <v>0.34288896395912044</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>'AZ splitter'!A23-'AZ splitter'!A51</f>
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B23">
         <v>35</v>
@@ -3348,11 +3462,11 @@
       </c>
       <c r="E23">
         <f>'AZ splitter'!E23-'AZ splitter'!E51</f>
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F23">
         <f>'AZ splitter'!F23-'AZ splitter'!F51</f>
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G23">
         <v>3</v>
@@ -3376,6 +3490,7 @@
         <v>1</v>
       </c>
       <c r="N23">
+        <f>IF(SUM(AD23:AG23) &gt;0,ROUND(AB23*(AD23*$Y$26+AE23*$Y$27+AF23*$Y$28+AG23*$Y$29)/SUM(AD23:AG23),0), 0)</f>
         <v>7</v>
       </c>
       <c r="O23">
@@ -3399,50 +3514,53 @@
       <c r="U23" t="s">
         <v>40</v>
       </c>
-      <c r="W23" t="str">
+      <c r="X23" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y23" s="2">
+        <f>SUMPRODUCT(AI:AI,AG:AG)/SUMPRODUCT(A:A,AG:AG)</f>
+        <v>0.4157303370786517</v>
+      </c>
+      <c r="Z23" s="2">
+        <f>SUMPRODUCT(AJ:AJ,AG:AG)/SUMPRODUCT(A:A,AG:AG)</f>
+        <v>0.27237504843084076</v>
+      </c>
+      <c r="AB23">
+        <v>7</v>
+      </c>
+      <c r="AC23" t="str">
+        <f>IF(N23&gt;A23,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE23">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X23">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y23">
-        <f>IF(B23&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA23">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF23">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI23" s="1">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="AD23" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ23" s="1">
+        <f t="shared" si="7"/>
         <v>4.5862068965517242</v>
       </c>
-      <c r="AF23" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG23" s="2">
-        <f>SUMPRODUCT(AC:AC,AA:AA)/SUMPRODUCT(A:A,AA:AA)</f>
-        <v>0.55639097744360899</v>
-      </c>
-      <c r="AH23" s="2">
-        <f>SUMPRODUCT(AD:AD,AA:AA)/SUMPRODUCT(A:A,AA:AA)</f>
-        <v>0.3645320197044335</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>'AZ splitter'!A24-'AZ splitter'!A52</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B24">
         <v>45</v>
@@ -3455,11 +3573,11 @@
       </c>
       <c r="E24">
         <f>'AZ splitter'!E24-'AZ splitter'!E52</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F24">
         <f>'AZ splitter'!F24-'AZ splitter'!F52</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G24">
         <v>3</v>
@@ -3483,6 +3601,7 @@
         <v>1</v>
       </c>
       <c r="N24">
+        <f>IF(SUM(AD24:AG24) &gt;0,ROUND(AB24*(AD24*$Y$26+AE24*$Y$27+AF24*$Y$28+AG24*$Y$29)/SUM(AD24:AG24),0), 0)</f>
         <v>3</v>
       </c>
       <c r="O24">
@@ -3506,41 +3625,44 @@
       <c r="U24" t="s">
         <v>40</v>
       </c>
-      <c r="W24" t="str">
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AB24">
+        <v>3</v>
+      </c>
+      <c r="AC24" t="str">
+        <f>IF(N24&gt;A24,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE24">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y24">
-        <f>IF(B24&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z24">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA24">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC24" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF24">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI24" s="1">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="AD24" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ24" s="1">
+        <f t="shared" si="7"/>
         <v>1.9655172413793103</v>
       </c>
-      <c r="AG24" s="2"/>
-      <c r="AH24" s="2"/>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>'AZ splitter'!A25-'AZ splitter'!A53</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B25">
         <v>55</v>
@@ -3553,11 +3675,11 @@
       </c>
       <c r="E25">
         <f>'AZ splitter'!E25-'AZ splitter'!E53</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F25">
         <f>'AZ splitter'!F25-'AZ splitter'!F53</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G25">
         <v>3</v>
@@ -3581,6 +3703,7 @@
         <v>1</v>
       </c>
       <c r="N25">
+        <f>IF(SUM(AD25:AG25) &gt;0,ROUND(AB25*(AD25*$Y$26+AE25*$Y$27+AF25*$Y$28+AG25*$Y$29)/SUM(AD25:AG25),0), 0)</f>
         <v>3</v>
       </c>
       <c r="O25">
@@ -3604,38 +3727,48 @@
       <c r="U25" t="s">
         <v>40</v>
       </c>
-      <c r="W25" t="str">
+      <c r="X25" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB25">
+        <v>3</v>
+      </c>
+      <c r="AC25" t="str">
+        <f>IF(N25&gt;A25,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE25">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X25">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y25">
-        <f>IF(B25&gt;50,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA25">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF25">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI25" s="1">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="AD25" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ25" s="1">
+        <f t="shared" si="7"/>
         <v>1.6725663716814159</v>
       </c>
-      <c r="AG25" s="2"/>
-      <c r="AH25" s="2"/>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>165</v>
       </c>
@@ -3676,6 +3809,7 @@
         <v>2</v>
       </c>
       <c r="N26">
+        <f>IF(SUM(AD26:AG26) &gt;0,ROUND(AB26*(AD26*$Y$26+AE26*$Y$27+AF26*$Y$28+AG26*$Y$29)/SUM(AD26:AG26),0), 0)</f>
         <v>0</v>
       </c>
       <c r="O26">
@@ -3699,36 +3833,48 @@
       <c r="U26" t="s">
         <v>41</v>
       </c>
-      <c r="W26" t="str">
+      <c r="X26" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="str">
+        <f>IF(N26&gt;A26,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE26">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y26">
-        <f>IF(B26&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z26">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC26" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF26">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD26" s="1">
+      <c r="AG26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI26" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>222</v>
       </c>
@@ -3769,7 +3915,8 @@
         <v>2</v>
       </c>
       <c r="N27">
-        <v>13</v>
+        <f>IF(SUM(AD27:AG27) &gt;0,ROUND(AB27*(AD27*$Y$26+AE27*$Y$27+AF27*$Y$28+AG27*$Y$29)/SUM(AD27:AG27),0), 0)</f>
+        <v>0</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -3792,36 +3939,48 @@
       <c r="U27" t="s">
         <v>43</v>
       </c>
-      <c r="W27" t="str">
+      <c r="X27" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>13</v>
+      </c>
+      <c r="AC27" t="str">
+        <f>IF(N27&gt;A27,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE27">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y27">
-        <f>IF(B27&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z27">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA27">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF27">
         <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="AD27" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG27">
         <f t="shared" si="5"/>
-        <v>0.50000000000000044</v>
-      </c>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>165</v>
       </c>
@@ -3862,6 +4021,7 @@
         <v>2</v>
       </c>
       <c r="N28">
+        <f>IF(SUM(AD28:AG28) &gt;0,ROUND(AB28*(AD28*$Y$26+AE28*$Y$27+AF28*$Y$28+AG28*$Y$29)/SUM(AD28:AG28),0), 0)</f>
         <v>0</v>
       </c>
       <c r="O28">
@@ -3885,41 +4045,51 @@
       <c r="U28" t="s">
         <v>42</v>
       </c>
-      <c r="W28" t="str">
+      <c r="X28" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="str">
+        <f>IF(N28&gt;A28,"WARN","")</f>
+        <v/>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE28">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="X28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y28">
-        <f>IF(B28&gt;50,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AA28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AC28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AD28" s="1">
+      <c r="AG28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AG28" s="1"/>
-      <c r="AH28" s="1"/>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI28" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>'AZ splitter'!A39</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="B29">
         <v>55</v>
@@ -3936,7 +4106,7 @@
       </c>
       <c r="F29">
         <f>'AZ splitter'!F39</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -3983,19 +4153,26 @@
       <c r="U29" t="s">
         <v>31</v>
       </c>
-      <c r="W29" t="str">
-        <f t="shared" si="0"/>
+      <c r="X29" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC29" t="str">
+        <f t="shared" ref="AC29:AC42" si="8">IF(N29&gt;A29,"WARN","")</f>
         <v/>
       </c>
-      <c r="AC29" s="1"/>
-      <c r="AD29" s="1"/>
-      <c r="AG29" s="1"/>
-      <c r="AH29" s="1"/>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>'AZ splitter'!A40</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B30">
         <v>25</v>
@@ -4008,11 +4185,11 @@
       </c>
       <c r="E30">
         <f>'AZ splitter'!E40</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <f>'AZ splitter'!F40</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -4059,19 +4236,19 @@
       <c r="U30" t="s">
         <v>44</v>
       </c>
-      <c r="W30" t="str">
-        <f t="shared" si="0"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AC30" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
-      <c r="AG30" s="1"/>
-      <c r="AH30" s="1"/>
-    </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI30" s="1"/>
+      <c r="AJ30" s="1"/>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>'AZ splitter'!A41</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B31">
         <v>35</v>
@@ -4084,11 +4261,11 @@
       </c>
       <c r="E31">
         <f>'AZ splitter'!E41</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <f>'AZ splitter'!F41</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -4135,17 +4312,17 @@
       <c r="U31" t="s">
         <v>44</v>
       </c>
-      <c r="W31" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC31" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
-    </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI31" s="1"/>
+      <c r="AJ31" s="1"/>
+    </row>
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>'AZ splitter'!A42</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B32">
         <v>45</v>
@@ -4158,11 +4335,11 @@
       </c>
       <c r="E32">
         <f>'AZ splitter'!E42</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <f>'AZ splitter'!F42</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -4209,17 +4386,17 @@
       <c r="U32" t="s">
         <v>44</v>
       </c>
-      <c r="W32" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC32" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="1"/>
+    </row>
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>'AZ splitter'!A43</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B33">
         <v>25</v>
@@ -4236,7 +4413,7 @@
       </c>
       <c r="F33">
         <f>'AZ splitter'!F43</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>2</v>
@@ -4283,17 +4460,17 @@
       <c r="U33" t="s">
         <v>34</v>
       </c>
-      <c r="W33" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC33" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI33" s="1"/>
+      <c r="AJ33" s="1"/>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>'AZ splitter'!A44</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B34">
         <v>35</v>
@@ -4310,7 +4487,7 @@
       </c>
       <c r="F34">
         <f>'AZ splitter'!F44</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>2</v>
@@ -4357,17 +4534,17 @@
       <c r="U34" t="s">
         <v>35</v>
       </c>
-      <c r="W34" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC34" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="1"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI34" s="1"/>
+      <c r="AJ34" s="1"/>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>'AZ splitter'!A45</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B35">
         <v>45</v>
@@ -4384,7 +4561,7 @@
       </c>
       <c r="F35">
         <f>'AZ splitter'!F45</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <v>2</v>
@@ -4431,17 +4608,17 @@
       <c r="U35" t="s">
         <v>36</v>
       </c>
-      <c r="W35" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC35" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC35" s="1"/>
-      <c r="AD35" s="1"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI35" s="1"/>
+      <c r="AJ35" s="1"/>
+    </row>
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>'AZ splitter'!A46</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B36">
         <v>55</v>
@@ -4458,7 +4635,7 @@
       </c>
       <c r="F36">
         <f>'AZ splitter'!F46</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>2</v>
@@ -4505,17 +4682,17 @@
       <c r="U36" t="s">
         <v>27</v>
       </c>
-      <c r="W36" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC36" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC36" s="1"/>
-      <c r="AD36" s="1"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI36" s="1"/>
+      <c r="AJ36" s="1"/>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>'AZ splitter'!A47</f>
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>25</v>
@@ -4532,7 +4709,7 @@
       </c>
       <c r="F37">
         <f>'AZ splitter'!F47</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G37">
         <v>3</v>
@@ -4579,17 +4756,17 @@
       <c r="U37" t="s">
         <v>37</v>
       </c>
-      <c r="W37" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC37" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC37" s="1"/>
-      <c r="AD37" s="1"/>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI37" s="1"/>
+      <c r="AJ37" s="1"/>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>'AZ splitter'!A48</f>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B38">
         <v>35</v>
@@ -4606,7 +4783,7 @@
       </c>
       <c r="F38">
         <f>'AZ splitter'!F48</f>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>3</v>
@@ -4653,17 +4830,17 @@
       <c r="U38" t="s">
         <v>38</v>
       </c>
-      <c r="W38" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC38" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>'AZ splitter'!A49</f>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="B39">
         <v>45</v>
@@ -4680,7 +4857,7 @@
       </c>
       <c r="F39">
         <f>'AZ splitter'!F49</f>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <v>3</v>
@@ -4727,17 +4904,17 @@
       <c r="U39" t="s">
         <v>39</v>
       </c>
-      <c r="W39" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC39" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC39" s="1"/>
-      <c r="AD39" s="1"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+    </row>
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>'AZ splitter'!A50</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B40">
         <v>25</v>
@@ -4750,11 +4927,11 @@
       </c>
       <c r="E40">
         <f>'AZ splitter'!E50</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F40">
         <f>'AZ splitter'!F50</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G40">
         <v>3</v>
@@ -4801,17 +4978,17 @@
       <c r="U40" t="s">
         <v>40</v>
       </c>
-      <c r="W40" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC40" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC40" s="1"/>
-      <c r="AD40" s="1"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="1"/>
+    </row>
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>'AZ splitter'!A51</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B41">
         <v>35</v>
@@ -4824,11 +5001,11 @@
       </c>
       <c r="E41">
         <f>'AZ splitter'!E51</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <f>'AZ splitter'!F51</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>3</v>
@@ -4875,17 +5052,17 @@
       <c r="U41" t="s">
         <v>40</v>
       </c>
-      <c r="W41" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC41" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC41" s="1"/>
-      <c r="AD41" s="1"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI41" s="1"/>
+      <c r="AJ41" s="1"/>
+    </row>
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>'AZ splitter'!A52</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B42">
         <v>45</v>
@@ -4898,11 +5075,11 @@
       </c>
       <c r="E42">
         <f>'AZ splitter'!E52</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F42">
         <f>'AZ splitter'!F52</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>3</v>
@@ -4949,17 +5126,17 @@
       <c r="U42" t="s">
         <v>40</v>
       </c>
-      <c r="W42" t="str">
-        <f t="shared" si="0"/>
+      <c r="AC42" t="str">
+        <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="AC42" s="1"/>
-      <c r="AD42" s="1"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AI42" s="1"/>
+      <c r="AJ42" s="1"/>
+    </row>
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>'AZ splitter'!A53</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B43">
         <v>55</v>
@@ -4972,11 +5149,11 @@
       </c>
       <c r="E43">
         <f>'AZ splitter'!E53</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <f>'AZ splitter'!F53</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G43">
         <v>3</v>
@@ -5038,10 +5215,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
@@ -6878,7 +7055,7 @@
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>ROUND(A2*pop_essential_2007_bau!$V$3,0)</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B30">
         <v>85</v>
@@ -6889,7 +7066,7 @@
       </c>
       <c r="F30">
         <f>ROUND(F2*pop_essential_2007_bau!$V$3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G30" t="s">
         <v>25</v>
@@ -6898,7 +7075,7 @@
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>ROUND(A3*pop_essential_2007_bau!$V$3,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B31">
         <v>95</v>
@@ -6909,7 +7086,7 @@
       </c>
       <c r="F31">
         <f>ROUND(F3*pop_essential_2007_bau!$V$3,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" t="s">
         <v>26</v>
@@ -6938,7 +7115,7 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>ROUND(A5*pop_essential_2007_bau!$V$3,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33">
         <v>65</v>
@@ -6958,7 +7135,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>ROUND(A6*pop_essential_2007_bau!$V$3,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B34">
         <v>55</v>
@@ -6969,7 +7146,7 @@
       </c>
       <c r="F34">
         <f>ROUND(F6*pop_essential_2007_bau!$V$3,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G34" t="s">
         <v>27</v>
@@ -6978,7 +7155,7 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>ROUND(A7*pop_essential_2007_bau!$V$3,0)</f>
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="B35">
         <v>65</v>
@@ -6989,7 +7166,7 @@
       </c>
       <c r="F35">
         <f>ROUND(F7*pop_essential_2007_bau!$V$3,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G35" t="s">
         <v>29</v>
@@ -6998,7 +7175,7 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>ROUND(A8*pop_essential_2007_bau!$V$3,0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B36">
         <v>65</v>
@@ -7009,7 +7186,7 @@
       </c>
       <c r="F36">
         <f>ROUND(F8*pop_essential_2007_bau!$V$3,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G36" t="s">
         <v>28</v>
@@ -7018,7 +7195,7 @@
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>ROUND(A9*pop_essential_2007_bau!$V$3,0)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="B37">
         <v>75</v>
@@ -7029,7 +7206,7 @@
       </c>
       <c r="F37">
         <f>ROUND(F9*pop_essential_2007_bau!$V$3,0)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G37" t="s">
         <v>30</v>
@@ -7038,7 +7215,7 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>ROUND(A10*pop_essential_2007_bau!$V$3,0)</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B38">
         <v>55</v>
@@ -7049,7 +7226,7 @@
       </c>
       <c r="F38">
         <f>ROUND(F10*pop_essential_2007_bau!$V$3,0)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G38" t="s">
         <v>31</v>
@@ -7058,7 +7235,7 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>ROUND(A11*pop_essential_2007_bau!$V$3,0)</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="B39">
         <v>55</v>
@@ -7069,7 +7246,7 @@
       </c>
       <c r="F39">
         <f>ROUND(F11*pop_essential_2007_bau!$V$3,0)</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G39" t="s">
         <v>31</v>
@@ -7078,18 +7255,18 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>ROUND(A12*pop_essential_2007_bau!$V$7,0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B40">
         <v>25</v>
       </c>
       <c r="E40">
         <f>ROUND(E12*pop_essential_2007_bau!$V$7,0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F40">
         <f>ROUND(F12*pop_essential_2007_bau!$V$7,0)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G40" t="s">
         <v>44</v>
@@ -7098,18 +7275,18 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>ROUND(A13*pop_essential_2007_bau!$V$7,0)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B41">
         <v>35</v>
       </c>
       <c r="E41">
         <f>ROUND(E13*pop_essential_2007_bau!$V$7,0)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <f>ROUND(F13*pop_essential_2007_bau!$V$7,0)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G41" t="s">
         <v>44</v>
@@ -7118,18 +7295,18 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>ROUND(A14*pop_essential_2007_bau!$V$7,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B42">
         <v>45</v>
       </c>
       <c r="E42">
         <f>ROUND(E14*pop_essential_2007_bau!$V$7,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F42">
         <f>ROUND(F14*pop_essential_2007_bau!$V$7,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G42" t="s">
         <v>44</v>
@@ -7138,7 +7315,7 @@
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>ROUND(A15*pop_essential_2007_bau!$V$3,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B43">
         <v>25</v>
@@ -7149,7 +7326,7 @@
       </c>
       <c r="F43">
         <f>ROUND(F15*pop_essential_2007_bau!$V$3,0)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G43" t="s">
         <v>34</v>
@@ -7158,7 +7335,7 @@
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>ROUND(A16*pop_essential_2007_bau!$V$3,0)</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B44">
         <v>35</v>
@@ -7169,7 +7346,7 @@
       </c>
       <c r="F44">
         <f>ROUND(F16*pop_essential_2007_bau!$V$3,0)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G44" t="s">
         <v>35</v>
@@ -7178,7 +7355,7 @@
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>ROUND(A17*pop_essential_2007_bau!$V$3,0)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B45">
         <v>45</v>
@@ -7189,7 +7366,7 @@
       </c>
       <c r="F45">
         <f>ROUND(F17*pop_essential_2007_bau!$V$3,0)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G45" t="s">
         <v>36</v>
@@ -7198,7 +7375,7 @@
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>ROUND(A18*pop_essential_2007_bau!$V$3,0)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B46">
         <v>55</v>
@@ -7209,7 +7386,7 @@
       </c>
       <c r="F46">
         <f>ROUND(F18*pop_essential_2007_bau!$V$3,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G46" t="s">
         <v>27</v>
@@ -7218,7 +7395,7 @@
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>ROUND(A19*pop_essential_2007_bau!$V$3,0)</f>
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B47">
         <v>25</v>
@@ -7229,7 +7406,7 @@
       </c>
       <c r="F47">
         <f>ROUND(F19*pop_essential_2007_bau!$V$3,0)</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G47" t="s">
         <v>37</v>
@@ -7238,7 +7415,7 @@
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>ROUND(A20*pop_essential_2007_bau!$V$3,0)</f>
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B48">
         <v>35</v>
@@ -7249,7 +7426,7 @@
       </c>
       <c r="F48">
         <f>ROUND(F20*pop_essential_2007_bau!$V$3,0)</f>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="G48" t="s">
         <v>38</v>
@@ -7258,7 +7435,7 @@
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <f>ROUND(A21*pop_essential_2007_bau!$V$3,0)</f>
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="B49">
         <v>45</v>
@@ -7269,7 +7446,7 @@
       </c>
       <c r="F49">
         <f>ROUND(F21*pop_essential_2007_bau!$V$3,0)</f>
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="G49" t="s">
         <v>39</v>
@@ -7278,18 +7455,18 @@
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>ROUND(A22*pop_essential_2007_bau!$V$5,0)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B50">
         <v>25</v>
       </c>
       <c r="E50">
         <f>ROUND(E22*pop_essential_2007_bau!$V$5,0)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F50">
         <f>ROUND(F22*pop_essential_2007_bau!$V$5,0)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G50" t="s">
         <v>40</v>
@@ -7298,18 +7475,18 @@
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>ROUND(A23*pop_essential_2007_bau!$V$5,0)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B51">
         <v>35</v>
       </c>
       <c r="E51">
         <f>ROUND(E23*pop_essential_2007_bau!$V$5,0)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F51">
         <f>ROUND(F23*pop_essential_2007_bau!$V$5,0)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G51" t="s">
         <v>40</v>
@@ -7318,18 +7495,18 @@
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <f>ROUND(A24*pop_essential_2007_bau!$V$5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B52">
         <v>45</v>
       </c>
       <c r="E52">
         <f>ROUND(E24*pop_essential_2007_bau!$V$5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F52">
         <f>ROUND(F24*pop_essential_2007_bau!$V$5,0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G52" t="s">
         <v>40</v>
@@ -7338,18 +7515,18 @@
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <f>ROUND(A25*pop_essential_2007_bau!$V$5,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B53">
         <v>55</v>
       </c>
       <c r="E53">
         <f>ROUND(E25*pop_essential_2007_bau!$V$5,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F53">
         <f>ROUND(F25*pop_essential_2007_bau!$V$5,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G53" t="s">
         <v>40</v>
@@ -7358,7 +7535,7 @@
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <f>ROUND(A26*pop_essential_2007_bau!$V$3,0)</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="B54">
         <v>5</v>
@@ -7378,7 +7555,7 @@
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <f>ROUND(A27*pop_essential_2007_bau!$V$3,0)</f>
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="B55">
         <v>15</v>
@@ -7389,7 +7566,7 @@
       </c>
       <c r="F55">
         <f>ROUND(F27*pop_essential_2007_bau!$V$3,0)</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G55" t="s">
         <v>43</v>
@@ -7398,7 +7575,7 @@
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>ROUND(A28*pop_essential_2007_bau!$V$3,0)</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="B56">
         <v>5</v>

</xml_diff>